<commit_message>
Update statistics for 10 DEZ
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Prozent Infras / Ops Tickets</t>
+  </si>
+  <si>
+    <t>19 NOV - 09 DEZ</t>
   </si>
 </sst>
 </file>
@@ -183,8 +186,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -298,7 +303,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="105">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -350,6 +355,7 @@
     <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -401,6 +407,7 @@
     <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,10 +453,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$J$1</c:f>
+              <c:f>stats!$D$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -470,16 +477,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>41961.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41982.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$J$33</c:f>
+              <c:f>stats!$D$33:$K$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -500,6 +510,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.697916666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -514,10 +527,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$J$1</c:f>
+              <c:f>stats!$D$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -538,16 +551,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>41961.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41982.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$J$34</c:f>
+              <c:f>stats!$D$34:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -568,6 +584,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.645833333333333</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,10 +601,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$J$1</c:f>
+              <c:f>stats!$D$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -606,16 +625,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>41961.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41982.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$J$25</c:f>
+              <c:f>stats!$D$25:$K$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -636,6 +658,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -653,11 +678,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2143670376"/>
-        <c:axId val="2143675464"/>
+        <c:axId val="2122004760"/>
+        <c:axId val="2065533384"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2143670376"/>
+        <c:axId val="2122004760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,14 +711,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143675464"/>
+        <c:crossAx val="2065533384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2143675464"/>
+        <c:axId val="2065533384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,10 +748,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143670376"/>
+        <c:crossAx val="2122004760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -873,11 +904,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2121786776"/>
-        <c:axId val="2121789752"/>
+        <c:axId val="2142335528"/>
+        <c:axId val="2142338504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121786776"/>
+        <c:axId val="2142335528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121789752"/>
+        <c:crossAx val="2142338504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -894,7 +925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121789752"/>
+        <c:axId val="2142338504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121786776"/>
+        <c:crossAx val="2142335528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -932,15 +963,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -961,10 +992,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="441146" cy="261610"/>
     <xdr:sp macro="" textlink="C33">
@@ -974,7 +1005,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6985000" y="8966200"/>
+          <a:off x="7505700" y="10566400"/>
           <a:ext cx="441146" cy="261610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1005,7 +1036,7 @@
           <a:fld id="{0D984E82-241E-B040-9441-E77404260ED3}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,75</a:t>
+            <a:t>0,77</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1015,10 +1046,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="434352" cy="261610"/>
     <xdr:sp macro="" textlink="C34">
@@ -1028,7 +1059,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6985000" y="9232900"/>
+          <a:off x="7505700" y="10807700"/>
           <a:ext cx="434352" cy="261610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1059,7 +1090,7 @@
           <a:fld id="{E5687BA9-F129-9348-BC57-1C2935757FF8}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,58</a:t>
+            <a:t>0,59</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1069,10 +1100,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="434352" cy="261610"/>
     <xdr:sp macro="" textlink="C25">
@@ -1082,7 +1113,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6985000" y="9486900"/>
+          <a:off x="7493000" y="11061700"/>
           <a:ext cx="434352" cy="261610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1113,7 +1144,7 @@
           <a:fld id="{35AB75BE-9053-C14B-966D-62C9AAE10ABF}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>1,89</a:t>
+            <a:t>1,79</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1123,10 +1154,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1531188" cy="307777"/>
     <xdr:sp macro="" textlink="">
@@ -1136,7 +1167,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7099300" y="8445500"/>
+          <a:off x="76200" y="8331200"/>
           <a:ext cx="1531188" cy="307777"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1175,16 +1206,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>787400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1530,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1539,7 +1570,7 @@
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" style="5" customWidth="1"/>
     <col min="4" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="2" customWidth="1"/>
+    <col min="10" max="11" width="13.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1570,6 +1601,9 @@
       <c r="J1" s="1">
         <v>41961</v>
       </c>
+      <c r="K1" s="1">
+        <v>41982</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
@@ -1595,6 +1629,9 @@
       </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1631,7 +1668,9 @@
       <c r="J4" s="2">
         <v>15</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
@@ -1657,6 +1696,9 @@
         <v>28</v>
       </c>
       <c r="J5" s="2">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2">
         <v>48</v>
       </c>
     </row>
@@ -1709,6 +1751,9 @@
       <c r="J9" s="2">
         <v>8</v>
       </c>
+      <c r="K9" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="B10" s="5" t="s">
@@ -1729,6 +1774,9 @@
       <c r="J10" s="2">
         <v>21</v>
       </c>
+      <c r="K10" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="B11" s="5" t="s">
@@ -1749,6 +1797,9 @@
       <c r="J11" s="2">
         <v>2</v>
       </c>
+      <c r="K11" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="D12" s="2">
@@ -1775,6 +1826,10 @@
       <c r="J12" s="2">
         <f>SUM(J9:J11)</f>
         <v>31</v>
+      </c>
+      <c r="K12" s="2">
+        <f>SUM(K9:K11)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1807,6 +1862,9 @@
       <c r="J14" s="2">
         <v>3.5</v>
       </c>
+      <c r="K14" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="B15" s="5" t="s">
@@ -1827,6 +1885,9 @@
       <c r="J15" s="2">
         <v>28</v>
       </c>
+      <c r="K15" s="2">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="B16" s="5" t="s">
@@ -1847,8 +1908,11 @@
       <c r="J16" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="D17" s="2">
         <v>44</v>
       </c>
@@ -1874,8 +1938,12 @@
         <f>SUM(J14:J16)</f>
         <v>33.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="2">
+        <f>SUM(K14:K16)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1900,8 +1968,11 @@
       <c r="J18" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1920,8 +1991,11 @@
       <c r="J19" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1929,7 +2003,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1957,8 +2031,11 @@
       <c r="J21" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -1975,7 +2052,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -1992,7 +2069,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2008,10 +2085,10 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="C25" s="2">
-        <f>AVERAGE(D25:J25)</f>
-        <v>1.8904761904761906</v>
+        <f>AVERAGE(D25:K25)</f>
+        <v>1.7916666666666667</v>
       </c>
       <c r="D25" s="2">
         <v>1.3</v>
@@ -2038,8 +2115,11 @@
         <f>AVERAGE(J22:J24)</f>
         <v>1.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2047,7 +2127,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2065,8 +2145,11 @@
       <c r="J27" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="B28" s="5" t="s">
         <v>13</v>
       </c>
@@ -2081,8 +2164,11 @@
       <c r="J28" s="2">
         <v>289</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" s="2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2096,8 +2182,12 @@
         <f>SUM(J27:J28)</f>
         <v>325</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="2">
+        <f>SUM(K27:K28)</f>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2105,7 +2195,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2113,8 +2203,8 @@
         <v>22</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D31:J31)</f>
-        <v>0.31177322528128976</v>
+        <f>AVERAGE(D31:K31)</f>
+        <v>0.31967657212112854</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" ref="D31:J31" si="0">(D18/D12)</f>
@@ -2144,8 +2234,12 @@
         <f t="shared" si="0"/>
         <v>0.22580645161290322</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" s="2">
+        <f t="shared" ref="K31" si="1">(K18/K12)</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="B32" s="5" t="s">
         <v>29</v>
       </c>
@@ -2153,97 +2247,109 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="1">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="2">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4516129032258063E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:10">
+      <c r="K32" s="2">
+        <f t="shared" ref="K32" si="3">(K19/K12)</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
       <c r="B33" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D33:J33)</f>
-        <v>0.75372042074935142</v>
+        <f>AVERAGE(D33:K33)</f>
+        <v>0.7688803681556825</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="2">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="4">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.69791666666666663</v>
       </c>
-    </row>
-    <row r="34" spans="2:10">
+      <c r="K33" s="2">
+        <f t="shared" ref="K33" si="5">K17/K5</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
       <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D34:J34)</f>
-        <v>0.58061470951079475</v>
+        <f>AVERAGE(D34:K34)</f>
+        <v>0.59137120415527877</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="3">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="6">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.64583333333333337</v>
       </c>
-    </row>
-    <row r="36" spans="2:10">
+      <c r="K34" s="2">
+        <f t="shared" ref="K34" si="7">K12/K5</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
       <c r="B36" s="5" t="s">
         <v>30</v>
       </c>
@@ -2263,8 +2369,12 @@
         <f>(J9/J12*100)</f>
         <v>25.806451612903224</v>
       </c>
-    </row>
-    <row r="37" spans="2:10">
+      <c r="K36" s="2">
+        <f>(K9/K12*100)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
       <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
@@ -2284,8 +2394,12 @@
         <f>(J10/J12*100)</f>
         <v>67.741935483870961</v>
       </c>
-    </row>
-    <row r="38" spans="2:10">
+      <c r="K37" s="2">
+        <f>(K10/K12*100)</f>
+        <v>53.125</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
@@ -2304,6 +2418,10 @@
       <c r="J38" s="2">
         <f>(J11/J12*100)</f>
         <v>6.4516129032258061</v>
+      </c>
+      <c r="K38" s="2">
+        <f>(K11/K12*100)</f>
+        <v>21.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update statistics and insights for 13 JAN 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19380" tabRatio="500"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>19 NOV - 09 DEZ</t>
+  </si>
+  <si>
+    <t>10 DEZ - 13 JAN</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -186,8 +192,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,7 +311,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="107">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -356,6 +364,7 @@
     <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -408,6 +417,7 @@
     <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,10 +463,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$K$1</c:f>
+              <c:f>stats!$D$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -480,16 +490,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>41982.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42017.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$K$33</c:f>
+              <c:f>stats!$D$33:$L$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -513,6 +526,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.953488372093023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -527,10 +543,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$K$1</c:f>
+              <c:f>stats!$D$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -554,16 +570,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>41982.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42017.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$K$34</c:f>
+              <c:f>stats!$D$34:$L$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -587,6 +606,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.790697674418605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -601,10 +623,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$K$1</c:f>
+              <c:f>stats!$D$1:$L$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -628,16 +650,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>41982.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42017.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$K$25</c:f>
+              <c:f>stats!$D$25:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -648,10 +673,10 @@
                   <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.15</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.783333333333333</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.6</c:v>
@@ -661,6 +686,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,11 +706,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2122004760"/>
-        <c:axId val="2065533384"/>
+        <c:axId val="-2136668840"/>
+        <c:axId val="-2136672088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2122004760"/>
+        <c:axId val="-2136668840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,14 +739,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065533384"/>
+        <c:crossAx val="-2136672088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2065533384"/>
+        <c:axId val="-2136672088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122004760"/>
+        <c:crossAx val="-2136668840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -816,10 +844,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$36:$J$36</c:f>
+              <c:f>stats!$G$36:$L$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>71.66666666666667</c:v>
                 </c:pt>
@@ -831,6 +859,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>25.80645161290322</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.23529411764706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,10 +879,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$37:$J$37</c:f>
+              <c:f>stats!$G$37:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>26.66666666666667</c:v>
                 </c:pt>
@@ -860,6 +894,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>67.74193548387096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.23529411764706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -874,10 +914,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$38:$J$38</c:f>
+              <c:f>stats!$G$38:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
@@ -889,6 +929,12 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.451612903225806</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.52941176470588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,11 +950,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2142335528"/>
-        <c:axId val="2142338504"/>
+        <c:axId val="-2063183400"/>
+        <c:axId val="-2063186392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142335528"/>
+        <c:axId val="-2063183400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -917,7 +963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142338504"/>
+        <c:crossAx val="-2063186392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -925,7 +971,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142338504"/>
+        <c:axId val="-2063186392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,7 +982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142335528"/>
+        <c:crossAx val="-2063183400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1036,7 +1082,7 @@
           <a:fld id="{0D984E82-241E-B040-9441-E77404260ED3}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,77</a:t>
+            <a:t>0,79</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1090,7 +1136,7 @@
           <a:fld id="{E5687BA9-F129-9348-BC57-1C2935757FF8}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,59</a:t>
+            <a:t>0,61</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1144,7 +1190,7 @@
           <a:fld id="{35AB75BE-9053-C14B-966D-62C9AAE10ABF}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>1,79</a:t>
+            <a:t>1,77</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1559,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1570,10 +1616,10 @@
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" style="5" customWidth="1"/>
     <col min="4" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="11" width="13.83203125" style="2" customWidth="1"/>
+    <col min="10" max="12" width="13.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1604,8 +1650,11 @@
       <c r="K1" s="1">
         <v>41982</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1">
+        <v>42017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1633,8 +1682,11 @@
       <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1642,7 +1694,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1671,8 +1723,11 @@
       <c r="K4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1701,8 +1756,11 @@
       <c r="K5" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1710,7 +1768,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +1779,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1729,7 +1787,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1754,8 +1812,11 @@
       <c r="K9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1777,8 +1838,11 @@
       <c r="K10" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1800,8 +1864,14 @@
       <c r="K11" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="2">
         <v>32</v>
       </c>
@@ -1831,8 +1901,12 @@
         <f>SUM(K9:K11)</f>
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="2">
+        <f>SUM(L9:L11)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1840,7 +1914,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1865,8 +1939,12 @@
       <c r="K14" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14" s="2">
+        <v>17.5</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
@@ -1888,8 +1966,11 @@
       <c r="K15" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="2">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -1911,8 +1992,14 @@
       <c r="K16" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D17" s="2">
         <v>44</v>
       </c>
@@ -1942,8 +2029,12 @@
         <f>SUM(K14:K16)</f>
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="2">
+        <f>SUM(L14:L16)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="B18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1971,8 +2062,11 @@
       <c r="K18" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1994,8 +2088,11 @@
       <c r="K19" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2003,7 +2100,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2034,8 +2131,11 @@
       <c r="K21" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2052,7 +2152,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:12">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2069,7 +2169,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:12">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2085,10 +2185,13 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:12">
+      <c r="B25" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="C25" s="2">
-        <f>AVERAGE(D25:K25)</f>
-        <v>1.7916666666666667</v>
+        <f>AVERAGE(D25:L25)</f>
+        <v>1.7666666666666666</v>
       </c>
       <c r="D25" s="2">
         <v>1.3</v>
@@ -2100,26 +2203,25 @@
         <v>1.9</v>
       </c>
       <c r="G25" s="2">
-        <f>AVERAGE(G22:G24)</f>
-        <v>3.1500000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="H25" s="2">
-        <f>AVERAGE(H22:H24)</f>
-        <v>1.7833333333333332</v>
+        <v>1.5</v>
       </c>
       <c r="I25" s="2">
-        <f>AVERAGE(I22:I24)</f>
         <v>1.6</v>
       </c>
       <c r="J25" s="2">
-        <f>AVERAGE(J22:J24)</f>
         <v>1.9</v>
       </c>
       <c r="K25" s="2">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" s="2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2127,7 +2229,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2148,8 +2250,11 @@
       <c r="K27" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="B28" s="5" t="s">
         <v>13</v>
       </c>
@@ -2167,8 +2272,11 @@
       <c r="K28" s="2">
         <v>298</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28" s="2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2186,8 +2294,12 @@
         <f>SUM(K27:K28)</f>
         <v>338</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29" s="2">
+        <f>SUM(L27:L28)</f>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2195,7 +2307,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2203,8 +2315,8 @@
         <v>22</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D31:K31)</f>
-        <v>0.31967657212112854</v>
+        <f>AVERAGE(D31:L31)</f>
+        <v>0.31356871770244105</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" ref="D31:J31" si="0">(D18/D12)</f>
@@ -2235,11 +2347,15 @@
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31" si="1">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="1">(K18/K12)</f>
         <v>0.375</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26470588235294118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="B32" s="5" t="s">
         <v>29</v>
       </c>
@@ -2263,17 +2379,21 @@
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32" si="3">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="3">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:11">
+      <c r="L32" s="2">
+        <f t="shared" si="3"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D33:K33)</f>
-        <v>0.7688803681556825</v>
+        <f>AVERAGE(D33:L33)</f>
+        <v>0.78939236859316475</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" ref="D33:J33" si="4">D17/D5</f>
@@ -2304,17 +2424,21 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33" si="5">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="5">K17/K5</f>
         <v>0.875</v>
       </c>
-    </row>
-    <row r="34" spans="2:11">
+      <c r="L33" s="2">
+        <f t="shared" si="5"/>
+        <v>0.95348837209302328</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D34:K34)</f>
-        <v>0.59137120415527877</v>
+        <f>AVERAGE(D34:L34)</f>
+        <v>0.61351858974009277</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" ref="D34:J34" si="6">D12/D5</f>
@@ -2345,11 +2469,15 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34" si="7">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="7">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="36" spans="2:11">
+      <c r="L34" s="2">
+        <f t="shared" si="7"/>
+        <v>0.79069767441860461</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" s="5" t="s">
         <v>30</v>
       </c>
@@ -2373,8 +2501,12 @@
         <f>(K9/K12*100)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="2:11">
+      <c r="L36" s="2">
+        <f>(L9/L12*100)</f>
+        <v>38.235294117647058</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
       <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
@@ -2398,8 +2530,12 @@
         <f>(K10/K12*100)</f>
         <v>53.125</v>
       </c>
-    </row>
-    <row r="38" spans="2:11">
+      <c r="L37" s="2">
+        <f>(L10/L12*100)</f>
+        <v>38.235294117647058</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
@@ -2422,6 +2558,10 @@
       <c r="K38" s="2">
         <f>(K11/K12*100)</f>
         <v>21.875</v>
+      </c>
+      <c r="L38" s="2">
+        <f>(L11/L12*100)</f>
+        <v>23.52941176470588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update statistics and insights for 03 FEB 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -46,9 +46,6 @@
     <t>In done column:</t>
   </si>
   <si>
-    <t>miscalculated estimations</t>
-  </si>
-  <si>
     <t>number of tickets</t>
   </si>
   <si>
@@ -128,6 +125,12 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>14 JAN - 03 FEB</t>
+  </si>
+  <si>
+    <t>Estimations</t>
   </si>
 </sst>
 </file>
@@ -192,8 +195,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,7 +318,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="111">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -365,6 +372,8 @@
     <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -418,6 +427,8 @@
     <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,10 +474,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$L$1</c:f>
+              <c:f>stats!$D$1:$M$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -493,16 +504,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>42017.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42038.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$L$33</c:f>
+              <c:f>stats!$D$33:$M$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -529,6 +543,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.953488372093023</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,10 +560,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$L$1</c:f>
+              <c:f>stats!$D$1:$M$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -573,16 +590,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>42017.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42038.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$L$34</c:f>
+              <c:f>stats!$D$34:$M$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -609,6 +629,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.790697674418605</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -623,10 +646,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$L$1</c:f>
+              <c:f>stats!$D$1:$M$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -653,16 +676,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>42017.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42038.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$L$25</c:f>
+              <c:f>stats!$D$25:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -689,6 +715,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -706,11 +735,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2136668840"/>
-        <c:axId val="-2136672088"/>
+        <c:axId val="2088098776"/>
+        <c:axId val="2088095560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2136668840"/>
+        <c:axId val="2088098776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,14 +768,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136672088"/>
+        <c:crossAx val="2088095560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2136672088"/>
+        <c:axId val="2088095560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,7 +805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136668840"/>
+        <c:crossAx val="2088098776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -844,10 +873,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$36:$L$36</c:f>
+              <c:f>stats!$G$36:$M$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>71.66666666666667</c:v>
                 </c:pt>
@@ -865,6 +894,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>38.23529411764706</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,10 +911,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$37:$L$37</c:f>
+              <c:f>stats!$G$37:$M$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>26.66666666666667</c:v>
                 </c:pt>
@@ -900,6 +932,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>38.23529411764706</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,10 +949,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$38:$L$38</c:f>
+              <c:f>stats!$G$38:$M$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
@@ -935,6 +970,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>23.52941176470588</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,11 +988,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2063183400"/>
-        <c:axId val="-2063186392"/>
+        <c:axId val="2107260456"/>
+        <c:axId val="2107263432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2063183400"/>
+        <c:axId val="2107260456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,7 +1001,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063186392"/>
+        <c:crossAx val="2107263432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -971,7 +1009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2063186392"/>
+        <c:axId val="2107263432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +1020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2063183400"/>
+        <c:crossAx val="2107260456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1607,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1616,7 +1654,7 @@
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" style="5" customWidth="1"/>
     <col min="4" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="12" width="13.83203125" style="2" customWidth="1"/>
+    <col min="10" max="13" width="13.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1624,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3">
         <v>41828</v>
@@ -1652,6 +1690,9 @@
       </c>
       <c r="L1" s="1">
         <v>42017</v>
+      </c>
+      <c r="M1" s="1">
+        <v>42038</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1659,31 +1700,34 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>34</v>
+      <c r="M2" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1726,6 +1770,9 @@
       <c r="L4" s="2">
         <v>17</v>
       </c>
+      <c r="M4" s="2">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
@@ -1758,6 +1805,9 @@
       </c>
       <c r="L5" s="2">
         <v>43</v>
+      </c>
+      <c r="M5" s="2">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1789,7 +1839,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -1815,6 +1865,9 @@
       <c r="L9" s="2">
         <v>13</v>
       </c>
+      <c r="M9" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="5" t="s">
@@ -1841,6 +1894,9 @@
       <c r="L10" s="2">
         <v>13</v>
       </c>
+      <c r="M10" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:13">
       <c r="B11" s="5" t="s">
@@ -1867,10 +1923,13 @@
       <c r="L11" s="2">
         <v>8</v>
       </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:13">
       <c r="B12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2">
         <v>32</v>
@@ -1882,28 +1941,32 @@
         <v>16</v>
       </c>
       <c r="G12" s="2">
-        <f>SUM(G9:G11)</f>
+        <f t="shared" ref="G12:M12" si="0">SUM(G9:G11)</f>
         <v>60</v>
       </c>
       <c r="H12" s="2">
-        <f>SUM(H9:H11)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="I12" s="2">
-        <f>SUM(I9:I11)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J12" s="2">
-        <f>SUM(J9:J11)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="K12" s="2">
-        <f>SUM(K9:K11)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="L12" s="2">
-        <f>SUM(L9:L11)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1916,7 +1979,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -1942,7 +2005,9 @@
       <c r="L14" s="2">
         <v>17.5</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="5" t="s">
@@ -1969,6 +2034,9 @@
       <c r="L15" s="2">
         <v>20.5</v>
       </c>
+      <c r="M15" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="5" t="s">
@@ -1995,10 +2063,13 @@
       <c r="L16" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2">
         <v>44</v>
@@ -2010,33 +2081,37 @@
         <v>33.5</v>
       </c>
       <c r="G17" s="2">
-        <f>SUM(G14:G16)</f>
+        <f t="shared" ref="G17:M17" si="1">SUM(G14:G16)</f>
         <v>54.5</v>
       </c>
       <c r="H17" s="2">
-        <f>SUM(H14:H16)</f>
+        <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
       <c r="I17" s="2">
-        <f>SUM(I14:I16)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J17" s="2">
-        <f>SUM(J14:J16)</f>
+        <f t="shared" si="1"/>
         <v>33.5</v>
       </c>
       <c r="K17" s="2">
-        <f>SUM(K14:K16)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="L17" s="2">
-        <f>SUM(L14:L16)</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="B18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2">
         <v>13</v>
@@ -2065,10 +2140,13 @@
       <c r="L18" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2091,8 +2169,11 @@
       <c r="L19" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2100,12 +2181,12 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="D21" s="4">
         <v>13</v>
@@ -2134,8 +2215,11 @@
       <c r="L21" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2152,7 +2236,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2169,7 +2253,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2185,9 +2269,9 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2">
         <f>AVERAGE(D25:L25)</f>
@@ -2220,8 +2304,11 @@
       <c r="L25" s="2">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="2">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2229,12 +2316,12 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2253,10 +2340,13 @@
       <c r="L27" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="B28" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2275,8 +2365,11 @@
       <c r="L28" s="2">
         <v>298</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2298,8 +2391,12 @@
         <f>SUM(L27:L28)</f>
         <v>338</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="2">
+        <f>SUM(M27:M28)</f>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2307,261 +2404,289 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2">
         <f>AVERAGE(D31:L31)</f>
         <v>0.31356871770244105</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:J31" si="0">(D18/D12)</f>
+        <f t="shared" ref="D31:J31" si="2">(D18/D12)</f>
         <v>0.40625</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31:L31" si="1">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="3">(K18/K12)</f>
         <v>0.375</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.26470588235294118</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="2">
+        <f t="shared" ref="M31" si="4">(M18/M12)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="B32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="2">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="5">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32:L32" si="3">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="6">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.8823529411764705E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:12">
+      <c r="M32" s="2">
+        <f t="shared" ref="M32" si="7">(M19/M12)</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
       <c r="B33" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="2">
         <f>AVERAGE(D33:L33)</f>
         <v>0.78939236859316475</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="4">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="8">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:L33" si="5">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="9">K17/K5</f>
         <v>0.875</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.95348837209302328</v>
       </c>
-    </row>
-    <row r="34" spans="2:12">
+      <c r="M33" s="2">
+        <f t="shared" ref="M33" si="10">M17/M5</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
       <c r="B34" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="2">
         <f>AVERAGE(D34:L34)</f>
         <v>0.61351858974009277</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="6">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="11">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34:L34" si="7">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="12">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>0.79069767441860461</v>
       </c>
-    </row>
-    <row r="36" spans="2:12">
+      <c r="M34" s="2">
+        <f t="shared" ref="M34" si="13">M12/M5</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13">
       <c r="B36" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" ref="G36:L36" si="14">(G9/G12*100)</f>
+        <v>71.666666666666671</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="14"/>
+        <v>30.76923076923077</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="14"/>
+        <v>60</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="14"/>
+        <v>25.806451612903224</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="14"/>
+        <v>25</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="14"/>
+        <v>38.235294117647058</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" ref="M36" si="15">(M9/M12*100)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="2">
-        <f>(G9/G12*100)</f>
-        <v>71.666666666666671</v>
-      </c>
-      <c r="H36" s="2">
-        <f>(H9/H12*100)</f>
-        <v>30.76923076923077</v>
-      </c>
-      <c r="I36" s="2">
-        <f>(I9/I12*100)</f>
-        <v>60</v>
-      </c>
-      <c r="J36" s="2">
-        <f>(J9/J12*100)</f>
-        <v>25.806451612903224</v>
-      </c>
-      <c r="K36" s="2">
-        <f>(K9/K12*100)</f>
-        <v>25</v>
-      </c>
-      <c r="L36" s="2">
-        <f>(L9/L12*100)</f>
+      <c r="G37" s="2">
+        <f t="shared" ref="G37:L37" si="16">(G10/G12*100)</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="16"/>
+        <v>34.615384615384613</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="16"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="16"/>
+        <v>67.741935483870961</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="16"/>
+        <v>53.125</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="16"/>
         <v>38.235294117647058</v>
       </c>
-    </row>
-    <row r="37" spans="2:12">
-      <c r="B37" s="5" t="s">
+      <c r="M37" s="2">
+        <f t="shared" ref="M37" si="17">(M10/M12*100)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G37" s="2">
-        <f>(G10/G12*100)</f>
+      <c r="G38" s="2">
+        <f t="shared" ref="G38:L38" si="18">(G11/G12*100)</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="18"/>
+        <v>34.615384615384613</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="18"/>
         <v>26.666666666666668</v>
       </c>
-      <c r="H37" s="2">
-        <f>(H10/H12*100)</f>
-        <v>34.615384615384613</v>
-      </c>
-      <c r="I37" s="2">
-        <f>(I10/I12*100)</f>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="J37" s="2">
-        <f>(J10/J12*100)</f>
-        <v>67.741935483870961</v>
-      </c>
-      <c r="K37" s="2">
-        <f>(K10/K12*100)</f>
-        <v>53.125</v>
-      </c>
-      <c r="L37" s="2">
-        <f>(L10/L12*100)</f>
-        <v>38.235294117647058</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12">
-      <c r="B38" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G38" s="2">
-        <f>(G11/G12*100)</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="H38" s="2">
-        <f>(H11/H12*100)</f>
-        <v>34.615384615384613</v>
-      </c>
-      <c r="I38" s="2">
-        <f>(I11/I12*100)</f>
-        <v>26.666666666666668</v>
-      </c>
       <c r="J38" s="2">
-        <f>(J11/J12*100)</f>
+        <f t="shared" si="18"/>
         <v>6.4516129032258061</v>
       </c>
       <c r="K38" s="2">
-        <f>(K11/K12*100)</f>
+        <f t="shared" si="18"/>
         <v>21.875</v>
       </c>
       <c r="L38" s="2">
-        <f>(L11/L12*100)</f>
+        <f t="shared" si="18"/>
         <v>23.52941176470588</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" ref="M38" si="19">(M11/M12*100)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Update statistics and insights for 24 FEB 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Estimations</t>
+  </si>
+  <si>
+    <t>04 FEB - 24 FEB</t>
   </si>
 </sst>
 </file>
@@ -195,8 +198,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,7 +325,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="115">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -374,6 +381,8 @@
     <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -429,6 +438,8 @@
     <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,10 +485,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$M$1</c:f>
+              <c:f>stats!$D$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -507,16 +518,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42038.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42059.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$M$33</c:f>
+              <c:f>stats!$D$33:$N$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -546,6 +560,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -560,10 +577,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$M$1</c:f>
+              <c:f>stats!$D$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -593,16 +610,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42038.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42059.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$M$34</c:f>
+              <c:f>stats!$D$34:$N$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -632,6 +652,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.514285714285714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,10 +669,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$M$1</c:f>
+              <c:f>stats!$D$1:$N$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -679,16 +702,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42038.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42059.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$M$25</c:f>
+              <c:f>stats!$D$25:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -718,6 +744,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,11 +764,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088098776"/>
-        <c:axId val="2088095560"/>
+        <c:axId val="2041888648"/>
+        <c:axId val="2041890680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2088098776"/>
+        <c:axId val="2041888648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,14 +797,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088095560"/>
+        <c:crossAx val="2041890680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2088095560"/>
+        <c:axId val="2041890680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,7 +834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088098776"/>
+        <c:crossAx val="2041888648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -873,10 +902,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$36:$M$36</c:f>
+              <c:f>stats!$G$36:$N$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>71.66666666666667</c:v>
                 </c:pt>
@@ -897,6 +926,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.22222222222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -911,10 +943,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$37:$M$37</c:f>
+              <c:f>stats!$G$37:$N$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>26.66666666666667</c:v>
                 </c:pt>
@@ -935,6 +967,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.77777777777779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,10 +984,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$38:$M$38</c:f>
+              <c:f>stats!$G$38:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
@@ -972,6 +1007,9 @@
                   <c:v>23.52941176470588</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -988,11 +1026,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2107260456"/>
-        <c:axId val="2107263432"/>
+        <c:axId val="2041969944"/>
+        <c:axId val="2041972920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2107260456"/>
+        <c:axId val="2041969944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,7 +1039,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107263432"/>
+        <c:crossAx val="2041972920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1009,7 +1047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107263432"/>
+        <c:axId val="2041972920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107260456"/>
+        <c:crossAx val="2041969944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1643,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1654,10 +1692,12 @@
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="3" width="21.6640625" style="5" customWidth="1"/>
     <col min="4" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="13" width="13.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
+    <col min="12" max="14" width="13.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1694,8 +1734,11 @@
       <c r="M1" s="1">
         <v>42038</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1">
+        <v>42059</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1729,8 +1772,11 @@
       <c r="M2" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1738,7 +1784,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1773,8 +1819,11 @@
       <c r="M4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1809,8 +1858,11 @@
       <c r="M5" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1818,7 +1870,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1829,7 +1881,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1837,7 +1889,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1868,8 +1920,11 @@
       <c r="M9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1897,8 +1952,11 @@
       <c r="M10" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1926,8 +1984,11 @@
       <c r="M11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1968,8 +2029,12 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" s="2">
+        <f t="shared" ref="N12" si="1">SUM(N9:N11)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1977,7 +2042,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2008,8 +2073,11 @@
       <c r="M14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2037,8 +2105,11 @@
       <c r="M15" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" s="2">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -2066,8 +2137,11 @@
       <c r="M16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2081,35 +2155,39 @@
         <v>33.5</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:M17" si="1">SUM(G14:G16)</f>
+        <f t="shared" ref="G17:M17" si="2">SUM(G14:G16)</f>
         <v>54.5</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.5</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="2">
+        <f t="shared" ref="N17" si="3">SUM(N14:N16)</f>
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2143,8 +2221,11 @@
       <c r="M18" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -2172,8 +2253,11 @@
       <c r="M19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2181,7 +2265,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2218,8 +2302,11 @@
       <c r="M21" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2323,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2253,7 +2340,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2269,7 +2356,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
@@ -2307,8 +2394,11 @@
       <c r="M25" s="2">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="2">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2316,7 +2406,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2343,8 +2433,11 @@
       <c r="M27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
@@ -2368,35 +2461,42 @@
       <c r="M28" s="2">
         <v>343</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
-        <f>SUM(I27:I28)</f>
+        <f t="shared" ref="I29:N29" si="4">SUM(I27:I28)</f>
         <v>317</v>
       </c>
       <c r="J29" s="2">
-        <f>SUM(J27:J28)</f>
+        <f t="shared" si="4"/>
         <v>325</v>
       </c>
       <c r="K29" s="2">
-        <f>SUM(K27:K28)</f>
+        <f t="shared" si="4"/>
         <v>338</v>
       </c>
       <c r="L29" s="2">
-        <f>SUM(L27:L28)</f>
+        <f t="shared" si="4"/>
         <v>338</v>
       </c>
       <c r="M29" s="2">
-        <f>SUM(M27:M28)</f>
+        <f t="shared" si="4"/>
         <v>369</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" s="2">
+        <f t="shared" si="4"/>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2404,7 +2504,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2416,47 +2516,51 @@
         <v>0.31356871770244105</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:J31" si="2">(D18/D12)</f>
+        <f t="shared" ref="D31:J31" si="5">(D18/D12)</f>
         <v>0.40625</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31:L31" si="3">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="6">(K18/K12)</f>
         <v>0.375</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.26470588235294118</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ref="M31" si="4">(M18/M12)</f>
+        <f t="shared" ref="M31:N31" si="7">(M18/M12)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="2">
+        <f t="shared" si="7"/>
+        <v>0.3888888888888889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="B32" s="5" t="s">
         <v>28</v>
       </c>
@@ -2464,35 +2568,39 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="5">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="8">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32:L32" si="6">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="9">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32" si="7">(M19/M12)</f>
+        <f t="shared" ref="M32:N32" si="10">(M19/M12)</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="33" spans="2:13">
+      <c r="N32" s="2">
+        <f t="shared" si="10"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
@@ -2501,47 +2609,51 @@
         <v>0.78939236859316475</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="8">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="11">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:L33" si="9">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="12">K17/K5</f>
         <v>0.875</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.95348837209302328</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33" si="10">M17/M5</f>
+        <f t="shared" ref="M33:N33" si="13">M17/M5</f>
         <v>0.375</v>
       </c>
-    </row>
-    <row r="34" spans="2:13">
+      <c r="N33" s="2">
+        <f t="shared" si="13"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14">
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
@@ -2550,142 +2662,158 @@
         <v>0.61351858974009277</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="11">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="14">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34:L34" si="12">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="15">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.79069767441860461</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34" si="13">M12/M5</f>
+        <f t="shared" ref="M34:N34" si="16">M12/M5</f>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="36" spans="2:13">
+      <c r="N34" s="2">
+        <f t="shared" si="16"/>
+        <v>0.51428571428571423</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14">
       <c r="B36" s="5" t="s">
         <v>29</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" ref="G36:L36" si="14">(G9/G12*100)</f>
+        <f t="shared" ref="G36:L36" si="17">(G9/G12*100)</f>
         <v>71.666666666666671</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>30.76923076923077</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>60</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>25.806451612903224</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>25</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" ref="M36" si="15">(M9/M12*100)</f>
+        <f t="shared" ref="M36:N36" si="18">(M9/M12*100)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="2:13">
+      <c r="N36" s="2">
+        <f t="shared" si="18"/>
+        <v>22.222222222222221</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
       <c r="B37" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" ref="G37:L37" si="16">(G10/G12*100)</f>
+        <f t="shared" ref="G37:L37" si="19">(G10/G12*100)</f>
         <v>26.666666666666668</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>13.333333333333334</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>67.741935483870961</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>53.125</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ref="M37" si="17">(M10/M12*100)</f>
+        <f t="shared" ref="M37:N37" si="20">(M10/M12*100)</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="38" spans="2:13">
+      <c r="N37" s="2">
+        <f t="shared" si="20"/>
+        <v>77.777777777777786</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
       <c r="B38" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ref="G38:L38" si="18">(G11/G12*100)</f>
+        <f t="shared" ref="G38:L38" si="21">(G11/G12*100)</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>26.666666666666668</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>6.4516129032258061</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>21.875</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>23.52941176470588</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" ref="M38" si="19">(M11/M12*100)</f>
+        <f t="shared" ref="M38:N38" si="22">(M11/M12*100)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update statistics and insights for 17 MAR 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>04 FEB - 24 FEB</t>
+  </si>
+  <si>
+    <t>25 FEB - 17 MAR</t>
+  </si>
+  <si>
+    <t>tracked pairing time in days</t>
   </si>
 </sst>
 </file>
@@ -198,8 +204,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -325,7 +337,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="121">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -383,6 +395,9 @@
     <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -440,6 +455,9 @@
     <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,10 +503,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$N$1</c:f>
+              <c:f>stats!$D$1:$O$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -521,16 +539,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42059.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42080.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$N$33</c:f>
+              <c:f>stats!$D$33:$O$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -563,6 +584,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.017241379310345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -577,10 +601,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$N$1</c:f>
+              <c:f>stats!$D$1:$O$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -613,16 +637,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42059.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42080.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$N$34</c:f>
+              <c:f>stats!$D$34:$O$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -655,6 +682,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.514285714285714</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.137931034482759</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -669,10 +699,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$N$1</c:f>
+              <c:f>stats!$D$1:$O$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -705,16 +735,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42059.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42080.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$N$25</c:f>
+              <c:f>stats!$D$25:$O$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -747,6 +780,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,11 +800,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2041888648"/>
-        <c:axId val="2041890680"/>
+        <c:axId val="-2137553560"/>
+        <c:axId val="-2137548312"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2041888648"/>
+        <c:axId val="-2137553560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,14 +833,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041890680"/>
+        <c:crossAx val="-2137548312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2041890680"/>
+        <c:axId val="-2137548312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041888648"/>
+        <c:crossAx val="-2137553560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -896,16 +932,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Bugs</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$36:$N$36</c:f>
+              <c:f>stats!$G$37:$O$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>71.66666666666667</c:v>
                 </c:pt>
@@ -929,6 +962,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>22.22222222222222</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66.66666666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,16 +973,13 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Features</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$37:$N$37</c:f>
+              <c:f>stats!$G$38:$O$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>26.66666666666667</c:v>
                 </c:pt>
@@ -970,6 +1003,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>77.77777777777779</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.27272727272727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -978,16 +1014,13 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>Infra / Ops</c:v>
-          </c:tx>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$38:$N$38</c:f>
+              <c:f>stats!$G$39:$O$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
@@ -1011,6 +1044,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.060606060606061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,11 +1062,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2041969944"/>
-        <c:axId val="2041972920"/>
+        <c:axId val="-2137459656"/>
+        <c:axId val="-2137456776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2041969944"/>
+        <c:axId val="-2137459656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1039,7 +1075,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041972920"/>
+        <c:crossAx val="-2137456776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1047,7 +1083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2041972920"/>
+        <c:axId val="-2137456776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +1094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2041969944"/>
+        <c:crossAx val="-2137459656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1086,13 +1122,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1116,7 +1152,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="441146" cy="261610"/>
@@ -1158,7 +1194,7 @@
           <a:fld id="{0D984E82-241E-B040-9441-E77404260ED3}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,79</a:t>
+            <a:t>0,77</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1170,7 +1206,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="434352" cy="261610"/>
@@ -1212,7 +1248,7 @@
           <a:fld id="{E5687BA9-F129-9348-BC57-1C2935757FF8}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,61</a:t>
+            <a:t>0,62</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1224,7 +1260,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="434352" cy="261610"/>
@@ -1266,7 +1302,7 @@
           <a:fld id="{35AB75BE-9053-C14B-966D-62C9AAE10ABF}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>1,77</a:t>
+            <a:t>1,84</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1278,7 +1314,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1531188" cy="307777"/>
@@ -1330,13 +1366,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1681,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1695,9 +1731,10 @@
     <col min="10" max="10" width="13.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
     <col min="12" max="14" width="13.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1737,8 +1774,11 @@
       <c r="N1" s="1">
         <v>42059</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="1">
+        <v>42080</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1775,8 +1815,11 @@
       <c r="N2" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1784,7 +1827,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1822,8 +1865,11 @@
       <c r="N4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1861,8 +1907,11 @@
       <c r="N5" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1870,7 +1919,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1881,7 +1930,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1889,7 +1938,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1923,8 +1972,11 @@
       <c r="N9" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1955,8 +2007,11 @@
       <c r="N10" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1987,8 +2042,11 @@
       <c r="N11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -2030,11 +2088,15 @@
         <v>8</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" ref="N12" si="1">SUM(N9:N11)</f>
+        <f t="shared" ref="N12:O12" si="1">SUM(N9:N11)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -2042,7 +2104,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2076,8 +2138,11 @@
       <c r="N14" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2108,8 +2173,11 @@
       <c r="N15" s="2">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -2140,8 +2208,11 @@
       <c r="N16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2183,11 +2254,15 @@
         <v>12</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" ref="N17" si="3">SUM(N14:N16)</f>
+        <f t="shared" ref="N17:O17" si="3">SUM(N14:N16)</f>
         <v>24.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17" s="2">
+        <f t="shared" si="3"/>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2224,8 +2299,11 @@
       <c r="N18" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -2256,8 +2334,11 @@
       <c r="N19" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2265,7 +2346,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2305,8 +2386,11 @@
       <c r="N21" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2323,7 +2407,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2340,7 +2424,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2356,13 +2440,13 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="2">
-        <f>AVERAGE(D25:L25)</f>
-        <v>1.7666666666666666</v>
+        <f>AVERAGE(D25:O25)</f>
+        <v>1.8374999999999997</v>
       </c>
       <c r="D25" s="2">
         <v>1.3</v>
@@ -2397,8 +2481,11 @@
       <c r="N25" s="2">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2406,7 +2493,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2436,8 +2523,11 @@
       <c r="N27" s="2">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="O27" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
@@ -2464,8 +2554,11 @@
       <c r="N28" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="O28" s="2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2495,8 +2588,12 @@
         <f t="shared" si="4"/>
         <v>387</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="O29" s="2">
+        <f t="shared" ref="O29" si="5">SUM(O27:O28)</f>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2504,7 +2601,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2512,55 +2609,59 @@
         <v>21</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D31:L31)</f>
-        <v>0.31356871770244105</v>
+        <f>AVERAGE(D31:O31)</f>
+        <v>0.32187687497716749</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:J31" si="5">(D18/D12)</f>
+        <f t="shared" ref="D31:J31" si="6">(D18/D12)</f>
         <v>0.40625</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.375</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31:L31" si="6">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="7">(K18/K12)</f>
         <v>0.375</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.26470588235294118</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ref="M31:N31" si="7">(M18/M12)</f>
+        <f t="shared" ref="M31:N31" si="8">(M18/M12)</f>
         <v>0.5</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.3888888888888889</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31" s="2">
+        <f t="shared" ref="O31" si="9">(O18/O12)</f>
+        <v>0.15151515151515152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="B32" s="5" t="s">
         <v>28</v>
       </c>
@@ -2568,253 +2669,292 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="8">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="10">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32:L32" si="9">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="11">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32:N32" si="10">(M19/M12)</f>
+        <f t="shared" ref="M32:N32" si="12">(M19/M12)</f>
         <v>0.125</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="33" spans="2:14">
+      <c r="O32" s="2">
+        <f t="shared" ref="O32" si="13">(O19/O12)</f>
+        <v>3.0303030303030304E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D33:L33)</f>
-        <v>0.78939236859316475</v>
+        <f>AVERAGE(D33:O33)</f>
+        <v>0.76639772472073575</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="11">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="14">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:L33" si="12">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="15">K17/K5</f>
         <v>0.875</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.95348837209302328</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33:N33" si="13">M17/M5</f>
+        <f t="shared" ref="M33:N33" si="16">M17/M5</f>
         <v>0.375</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.7</v>
       </c>
-    </row>
-    <row r="34" spans="2:14">
+      <c r="O33" s="2">
+        <f t="shared" ref="O33" si="17">O17/O5</f>
+        <v>1.0172413793103448</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D34:L34)</f>
-        <v>0.61351858974009277</v>
+        <f>AVERAGE(D34:O34)</f>
+        <v>0.61865700470244234</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="14">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="18">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34:L34" si="15">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="19">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.79069767441860461</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34:N34" si="16">M12/M5</f>
+        <f t="shared" ref="M34:N34" si="20">M12/M5</f>
         <v>0.25</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.51428571428571423</v>
       </c>
-    </row>
-    <row r="36" spans="2:14">
-      <c r="B36" s="5" t="s">
+      <c r="O34" s="2">
+        <f t="shared" ref="O34" si="21">O12/O5</f>
+        <v>1.1379310344827587</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
+      <c r="B35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="O35" s="2">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
+      <c r="B37" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="2">
-        <f t="shared" ref="G36:L36" si="17">(G9/G12*100)</f>
+      <c r="G37" s="2">
+        <f t="shared" ref="G37:L37" si="22">(G9/G12*100)</f>
         <v>71.666666666666671</v>
       </c>
-      <c r="H36" s="2">
-        <f t="shared" si="17"/>
+      <c r="H37" s="2">
+        <f t="shared" si="22"/>
         <v>30.76923076923077</v>
       </c>
-      <c r="I36" s="2">
-        <f t="shared" si="17"/>
+      <c r="I37" s="2">
+        <f t="shared" si="22"/>
         <v>60</v>
       </c>
-      <c r="J36" s="2">
-        <f t="shared" si="17"/>
+      <c r="J37" s="2">
+        <f t="shared" si="22"/>
         <v>25.806451612903224</v>
       </c>
-      <c r="K36" s="2">
-        <f t="shared" si="17"/>
+      <c r="K37" s="2">
+        <f t="shared" si="22"/>
         <v>25</v>
       </c>
-      <c r="L36" s="2">
-        <f t="shared" si="17"/>
+      <c r="L37" s="2">
+        <f t="shared" si="22"/>
         <v>38.235294117647058</v>
       </c>
-      <c r="M36" s="2">
-        <f t="shared" ref="M36:N36" si="18">(M9/M12*100)</f>
+      <c r="M37" s="2">
+        <f t="shared" ref="M37:N37" si="23">(M9/M12*100)</f>
         <v>25</v>
       </c>
-      <c r="N36" s="2">
-        <f t="shared" si="18"/>
+      <c r="N37" s="2">
+        <f t="shared" si="23"/>
         <v>22.222222222222221</v>
       </c>
-    </row>
-    <row r="37" spans="2:14">
-      <c r="B37" s="5" t="s">
+      <c r="O37" s="2">
+        <f t="shared" ref="O37" si="24">(O9/O12*100)</f>
+        <v>66.666666666666657</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15">
+      <c r="B38" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G37" s="2">
-        <f t="shared" ref="G37:L37" si="19">(G10/G12*100)</f>
+      <c r="G38" s="2">
+        <f t="shared" ref="G38:L38" si="25">(G10/G12*100)</f>
         <v>26.666666666666668</v>
       </c>
-      <c r="H37" s="2">
-        <f t="shared" si="19"/>
+      <c r="H38" s="2">
+        <f t="shared" si="25"/>
         <v>34.615384615384613</v>
       </c>
-      <c r="I37" s="2">
-        <f t="shared" si="19"/>
+      <c r="I38" s="2">
+        <f t="shared" si="25"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="J37" s="2">
-        <f t="shared" si="19"/>
+      <c r="J38" s="2">
+        <f t="shared" si="25"/>
         <v>67.741935483870961</v>
       </c>
-      <c r="K37" s="2">
-        <f t="shared" si="19"/>
+      <c r="K38" s="2">
+        <f t="shared" si="25"/>
         <v>53.125</v>
       </c>
-      <c r="L37" s="2">
-        <f t="shared" si="19"/>
+      <c r="L38" s="2">
+        <f t="shared" si="25"/>
         <v>38.235294117647058</v>
       </c>
-      <c r="M37" s="2">
-        <f t="shared" ref="M37:N37" si="20">(M10/M12*100)</f>
+      <c r="M38" s="2">
+        <f t="shared" ref="M38:N38" si="26">(M10/M12*100)</f>
         <v>75</v>
       </c>
-      <c r="N37" s="2">
-        <f t="shared" si="20"/>
+      <c r="N38" s="2">
+        <f t="shared" si="26"/>
         <v>77.777777777777786</v>
       </c>
-    </row>
-    <row r="38" spans="2:14">
-      <c r="B38" s="5" t="s">
+      <c r="O38" s="2">
+        <f t="shared" ref="O38" si="27">(O10/O12*100)</f>
+        <v>27.27272727272727</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
+      <c r="B39" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G38" s="2">
-        <f t="shared" ref="G38:L38" si="21">(G11/G12*100)</f>
+      <c r="G39" s="2">
+        <f t="shared" ref="G39:L39" si="28">(G11/G12*100)</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="H38" s="2">
-        <f t="shared" si="21"/>
+      <c r="H39" s="2">
+        <f t="shared" si="28"/>
         <v>34.615384615384613</v>
       </c>
-      <c r="I38" s="2">
-        <f t="shared" si="21"/>
+      <c r="I39" s="2">
+        <f t="shared" si="28"/>
         <v>26.666666666666668</v>
       </c>
-      <c r="J38" s="2">
-        <f t="shared" si="21"/>
+      <c r="J39" s="2">
+        <f t="shared" si="28"/>
         <v>6.4516129032258061</v>
       </c>
-      <c r="K38" s="2">
-        <f t="shared" si="21"/>
+      <c r="K39" s="2">
+        <f t="shared" si="28"/>
         <v>21.875</v>
       </c>
-      <c r="L38" s="2">
-        <f t="shared" si="21"/>
+      <c r="L39" s="2">
+        <f t="shared" si="28"/>
         <v>23.52941176470588</v>
       </c>
-      <c r="M38" s="2">
-        <f t="shared" ref="M38:N38" si="22">(M11/M12*100)</f>
+      <c r="M39" s="2">
+        <f t="shared" ref="M39:N39" si="29">(M11/M12*100)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="2">
-        <f t="shared" si="22"/>
+      <c r="N39" s="2">
+        <f t="shared" si="29"/>
         <v>0</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" ref="O39" si="30">(O11/O12*100)</f>
+        <v>6.0606060606060606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update statistics and insights for 07 APR 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>tracked pairing time in days</t>
+  </si>
+  <si>
+    <t>18 MAR - 07 APR</t>
   </si>
 </sst>
 </file>
@@ -204,8 +207,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -337,7 +342,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="123">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -398,6 +403,7 @@
     <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -458,6 +464,7 @@
     <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -503,10 +510,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$O$1</c:f>
+              <c:f>stats!$D$1:$P$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -542,16 +549,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42080.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42101.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$O$33</c:f>
+              <c:f>stats!$D$33:$P$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -587,6 +597,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.017241379310345</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -601,10 +614,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$O$1</c:f>
+              <c:f>stats!$D$1:$P$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -640,16 +653,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42080.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42101.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$O$34</c:f>
+              <c:f>stats!$D$34:$P$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -685,6 +701,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.137931034482759</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -699,10 +718,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$O$1</c:f>
+              <c:f>stats!$D$1:$P$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -738,16 +757,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42080.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42101.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$O$25</c:f>
+              <c:f>stats!$D$25:$P$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -783,6 +805,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -800,11 +825,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137553560"/>
-        <c:axId val="-2137548312"/>
+        <c:axId val="2115649320"/>
+        <c:axId val="2115655272"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2137553560"/>
+        <c:axId val="2115649320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,14 +858,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137548312"/>
+        <c:crossAx val="2115655272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2137548312"/>
+        <c:axId val="2115655272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137553560"/>
+        <c:crossAx val="2115649320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -935,10 +960,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$37:$O$37</c:f>
+              <c:f>stats!$G$37:$P$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>71.66666666666667</c:v>
                 </c:pt>
@@ -965,6 +990,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>66.66666666666665</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71.42857142857143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,10 +1004,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$38:$O$38</c:f>
+              <c:f>stats!$G$38:$P$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>26.66666666666667</c:v>
                 </c:pt>
@@ -1006,6 +1034,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>27.27272727272727</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.57142857142857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,10 +1048,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$39:$O$39</c:f>
+              <c:f>stats!$G$39:$P$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
@@ -1047,6 +1078,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>6.060606060606061</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1062,11 +1096,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2137459656"/>
-        <c:axId val="-2137456776"/>
+        <c:axId val="2115713240"/>
+        <c:axId val="2115716168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2137459656"/>
+        <c:axId val="2115713240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,7 +1109,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137456776"/>
+        <c:crossAx val="2115716168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1083,7 +1117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137456776"/>
+        <c:axId val="2115716168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,7 +1128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137459656"/>
+        <c:crossAx val="2115713240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1248,7 +1282,7 @@
           <a:fld id="{E5687BA9-F129-9348-BC57-1C2935757FF8}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,62</a:t>
+            <a:t>0,60</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1302,7 +1336,7 @@
           <a:fld id="{35AB75BE-9053-C14B-966D-62C9AAE10ABF}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>1,84</a:t>
+            <a:t>1,87</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1717,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1731,10 +1765,10 @@
     <col min="10" max="10" width="13.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
     <col min="12" max="14" width="13.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" style="2" customWidth="1"/>
+    <col min="15" max="16" width="14.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1777,8 +1811,11 @@
       <c r="O1" s="1">
         <v>42080</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1">
+        <v>42101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1818,8 +1855,11 @@
       <c r="O2" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1827,7 +1867,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1868,8 +1908,11 @@
       <c r="O4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1910,8 +1953,11 @@
       <c r="O5" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1919,7 +1965,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1930,7 +1976,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1938,7 +1984,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1975,8 +2021,11 @@
       <c r="O9" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -2010,8 +2059,11 @@
       <c r="O10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2045,8 +2097,11 @@
       <c r="O11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -2095,8 +2150,12 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="2">
+        <f t="shared" ref="P12" si="2">SUM(P9:P11)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -2104,7 +2163,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2141,8 +2200,11 @@
       <c r="O14" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2176,8 +2238,11 @@
       <c r="O15" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" s="2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -2211,8 +2276,11 @@
       <c r="O16" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2226,43 +2294,47 @@
         <v>33.5</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:M17" si="2">SUM(G14:G16)</f>
+        <f t="shared" ref="G17:M17" si="3">SUM(G14:G16)</f>
         <v>54.5</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33.5</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" ref="N17:O17" si="3">SUM(N14:N16)</f>
+        <f t="shared" ref="N17:O17" si="4">SUM(N14:N16)</f>
         <v>24.5</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17" s="2">
+        <f t="shared" ref="P17" si="5">SUM(P14:P16)</f>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2302,8 +2374,11 @@
       <c r="O18" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -2337,8 +2412,11 @@
       <c r="O19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2346,7 +2424,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2389,8 +2467,11 @@
       <c r="O21" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2407,7 +2488,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:16">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2424,7 +2505,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:16">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2440,13 +2521,13 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:16">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="2">
-        <f>AVERAGE(D25:O25)</f>
-        <v>1.8374999999999997</v>
+        <f>AVERAGE(D25:P25)</f>
+        <v>1.8653846153846152</v>
       </c>
       <c r="D25" s="2">
         <v>1.3</v>
@@ -2484,8 +2565,11 @@
       <c r="O25" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2493,7 +2577,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2526,8 +2610,11 @@
       <c r="O27" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
@@ -2557,43 +2644,50 @@
       <c r="O28" s="2">
         <v>373</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28" s="2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
-        <f t="shared" ref="I29:N29" si="4">SUM(I27:I28)</f>
+        <f t="shared" ref="I29:N29" si="6">SUM(I27:I28)</f>
         <v>317</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>325</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>338</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>338</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>369</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>387</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" ref="O29" si="5">SUM(O27:O28)</f>
+        <f t="shared" ref="O29:P29" si="7">SUM(O27:O28)</f>
         <v>409</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29" s="2">
+        <f t="shared" si="7"/>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2601,7 +2695,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2609,59 +2703,63 @@
         <v>21</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D31:O31)</f>
-        <v>0.32187687497716749</v>
+        <f>AVERAGE(D31:P31)</f>
+        <v>0.34107315931958315</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:J31" si="6">(D18/D12)</f>
+        <f t="shared" ref="D31:J31" si="8">(D18/D12)</f>
         <v>0.40625</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.375</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31:L31" si="7">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="9">(K18/K12)</f>
         <v>0.375</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.26470588235294118</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ref="M31:N31" si="8">(M18/M12)</f>
+        <f t="shared" ref="M31:N31" si="10">(M18/M12)</f>
         <v>0.5</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.3888888888888889</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" ref="O31" si="9">(O18/O12)</f>
+        <f t="shared" ref="O31:P31" si="11">(O18/O12)</f>
         <v>0.15151515151515152</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31" s="2">
+        <f t="shared" si="11"/>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="B32" s="5" t="s">
         <v>28</v>
       </c>
@@ -2669,157 +2767,169 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="10">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="12">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32:L32" si="11">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="13">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32:N32" si="12">(M19/M12)</f>
+        <f t="shared" ref="M32:N32" si="14">(M19/M12)</f>
         <v>0.125</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" ref="O32" si="13">(O19/O12)</f>
+        <f t="shared" ref="O32:P32" si="15">(O19/O12)</f>
         <v>3.0303030303030304E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:15">
+      <c r="P32" s="2">
+        <f t="shared" si="15"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D33:O33)</f>
-        <v>0.76639772472073575</v>
+        <f>AVERAGE(D33:P33)</f>
+        <v>0.77090559204990983</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="14">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="16">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:L33" si="15">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="17">K17/K5</f>
         <v>0.875</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.95348837209302328</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33:N33" si="16">M17/M5</f>
+        <f t="shared" ref="M33:N33" si="18">M17/M5</f>
         <v>0.375</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.7</v>
       </c>
       <c r="O33" s="2">
-        <f t="shared" ref="O33" si="17">O17/O5</f>
+        <f t="shared" ref="O33:P33" si="19">O17/O5</f>
         <v>1.0172413793103448</v>
       </c>
-    </row>
-    <row r="34" spans="2:15">
+      <c r="P33" s="2">
+        <f t="shared" si="19"/>
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16">
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D34:O34)</f>
-        <v>0.61865700470244234</v>
+        <f>AVERAGE(D34:P34)</f>
+        <v>0.59799108126379286</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="18">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="20">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34:L34" si="19">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="21">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.79069767441860461</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34:N34" si="20">M12/M5</f>
+        <f t="shared" ref="M34:N34" si="22">M12/M5</f>
         <v>0.25</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="O34" s="2">
-        <f t="shared" ref="O34" si="21">O12/O5</f>
+        <f t="shared" ref="O34:P34" si="23">O12/O5</f>
         <v>1.1379310344827587</v>
       </c>
-    </row>
-    <row r="35" spans="2:15">
+      <c r="P34" s="2">
+        <f t="shared" si="23"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -2833,128 +2943,143 @@
       <c r="O35" s="2">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="37" spans="2:15">
+      <c r="P35" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16">
       <c r="B37" s="5" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" ref="G37:L37" si="22">(G9/G12*100)</f>
+        <f t="shared" ref="G37:L37" si="24">(G9/G12*100)</f>
         <v>71.666666666666671</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>30.76923076923077</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>60</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>25.806451612903224</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>25</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ref="M37:N37" si="23">(M9/M12*100)</f>
+        <f t="shared" ref="M37:N37" si="25">(M9/M12*100)</f>
         <v>25</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>22.222222222222221</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" ref="O37" si="24">(O9/O12*100)</f>
+        <f t="shared" ref="O37:P37" si="26">(O9/O12*100)</f>
         <v>66.666666666666657</v>
       </c>
-    </row>
-    <row r="38" spans="2:15">
+      <c r="P37" s="2">
+        <f t="shared" si="26"/>
+        <v>71.428571428571431</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16">
       <c r="B38" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ref="G38:L38" si="25">(G10/G12*100)</f>
+        <f t="shared" ref="G38:L38" si="27">(G10/G12*100)</f>
         <v>26.666666666666668</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>13.333333333333334</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>67.741935483870961</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>53.125</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" ref="M38:N38" si="26">(M10/M12*100)</f>
+        <f t="shared" ref="M38:N38" si="28">(M10/M12*100)</f>
         <v>75</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>77.777777777777786</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" ref="O38" si="27">(O10/O12*100)</f>
+        <f t="shared" ref="O38:P38" si="29">(O10/O12*100)</f>
         <v>27.27272727272727</v>
       </c>
-    </row>
-    <row r="39" spans="2:15">
+      <c r="P38" s="2">
+        <f t="shared" si="29"/>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16">
       <c r="B39" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" ref="G39:L39" si="28">(G11/G12*100)</f>
+        <f t="shared" ref="G39:L39" si="30">(G11/G12*100)</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>26.666666666666668</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>6.4516129032258061</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>21.875</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>23.52941176470588</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" ref="M39:N39" si="29">(M11/M12*100)</f>
+        <f t="shared" ref="M39:N39" si="31">(M11/M12*100)</f>
         <v>0</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" ref="O39" si="30">(O11/O12*100)</f>
+        <f t="shared" ref="O39:P39" si="32">(O11/O12*100)</f>
         <v>6.0606060606060606</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="32"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update statistics and insights for 28 APR 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>18 MAR - 07 APR</t>
+  </si>
+  <si>
+    <t>08 APR - 28 APR</t>
   </si>
 </sst>
 </file>
@@ -207,8 +210,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -342,7 +347,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="125">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -404,6 +409,7 @@
     <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -465,6 +471,7 @@
     <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,10 +517,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$P$1</c:f>
+              <c:f>stats!$D$1:$Q$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -552,16 +559,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>42101.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42123.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$33:$P$33</c:f>
+              <c:f>stats!$D$33:$Q$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.758620689655172</c:v>
                 </c:pt>
@@ -600,6 +610,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.825</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.833333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,10 +627,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$P$1</c:f>
+              <c:f>stats!$D$1:$Q$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -656,16 +669,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>42101.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42123.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$34:$P$34</c:f>
+              <c:f>stats!$D$34:$Q$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.551724137931034</c:v>
                 </c:pt>
@@ -704,6 +720,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.259259259259259</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -718,10 +737,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>stats!$D$1:$P$1</c:f>
+              <c:f>stats!$D$1:$Q$1</c:f>
               <c:numCache>
                 <c:formatCode>dd/mm/yyyy</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>41828.0</c:v>
                 </c:pt>
@@ -760,16 +779,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>42101.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42123.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>stats!$D$25:$P$25</c:f>
+              <c:f>stats!$D$25:$Q$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1.3</c:v>
                 </c:pt>
@@ -808,6 +830,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,11 +850,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115649320"/>
-        <c:axId val="2115655272"/>
+        <c:axId val="2124147016"/>
+        <c:axId val="2124152040"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2115649320"/>
+        <c:axId val="2124147016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,14 +883,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115655272"/>
+        <c:crossAx val="2124152040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2115655272"/>
+        <c:axId val="2124152040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +920,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115649320"/>
+        <c:crossAx val="2124147016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -960,10 +985,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$37:$P$37</c:f>
+              <c:f>stats!$G$37:$Q$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>71.66666666666667</c:v>
                 </c:pt>
@@ -993,6 +1018,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>71.42857142857143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.57142857142857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,10 +1032,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$38:$P$38</c:f>
+              <c:f>stats!$G$38:$Q$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>26.66666666666667</c:v>
                 </c:pt>
@@ -1037,6 +1065,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>28.57142857142857</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71.42857142857143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1048,10 +1079,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>stats!$G$39:$P$39</c:f>
+              <c:f>stats!$G$39:$Q$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.666666666666667</c:v>
                 </c:pt>
@@ -1080,6 +1111,9 @@
                   <c:v>6.060606060606061</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1096,11 +1130,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2115713240"/>
-        <c:axId val="2115716168"/>
+        <c:axId val="2124191208"/>
+        <c:axId val="2124194088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115713240"/>
+        <c:axId val="2124191208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1109,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115716168"/>
+        <c:crossAx val="2124194088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1117,7 +1151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115716168"/>
+        <c:axId val="2124194088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1162,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115713240"/>
+        <c:crossAx val="2124191208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1228,7 +1262,7 @@
           <a:fld id="{0D984E82-241E-B040-9441-E77404260ED3}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,77</a:t>
+            <a:t>0,78</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1282,7 +1316,7 @@
           <a:fld id="{E5687BA9-F129-9348-BC57-1C2935757FF8}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,60</a:t>
+            <a:t>0,57</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1297,7 +1331,7 @@
       <xdr:row>59</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="434352" cy="261610"/>
+    <xdr:ext cx="441146" cy="261610"/>
     <xdr:sp macro="" textlink="C25">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="Textfeld 6"/>
@@ -1305,8 +1339,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7493000" y="11061700"/>
-          <a:ext cx="434352" cy="261610"/>
+          <a:off x="7493000" y="11252200"/>
+          <a:ext cx="441146" cy="261610"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1336,7 +1370,7 @@
           <a:fld id="{35AB75BE-9053-C14B-966D-62C9AAE10ABF}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>1,87</a:t>
+            <a:t>1,95</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1399,15 +1433,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1751,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1765,10 +1799,10 @@
     <col min="10" max="10" width="13.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
     <col min="12" max="14" width="13.83203125" style="2" customWidth="1"/>
-    <col min="15" max="16" width="14.33203125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="14.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1814,8 +1848,11 @@
       <c r="P1" s="1">
         <v>42101</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1">
+        <v>42123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1858,8 +1895,11 @@
       <c r="P2" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1867,7 +1907,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1911,8 +1951,11 @@
       <c r="P4" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1956,8 +1999,11 @@
       <c r="P5" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1965,7 +2011,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1976,7 +2022,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1984,7 +2030,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2024,8 +2070,11 @@
       <c r="P9" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -2062,8 +2111,11 @@
       <c r="P10" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2100,8 +2152,11 @@
       <c r="P11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -2151,11 +2206,15 @@
         <v>33</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" ref="P12" si="2">SUM(P9:P11)</f>
+        <f t="shared" ref="P12:Q12" si="2">SUM(P9:P11)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -2163,7 +2222,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2203,8 +2262,11 @@
       <c r="P14" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2241,8 +2303,11 @@
       <c r="P15" s="2">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="2">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -2279,8 +2344,11 @@
       <c r="P16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2330,11 +2398,15 @@
         <v>29.5</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" ref="P17" si="5">SUM(P14:P16)</f>
+        <f t="shared" ref="P17:Q17" si="5">SUM(P14:P16)</f>
         <v>16.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="2">
+        <f t="shared" si="5"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2377,8 +2449,11 @@
       <c r="P18" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -2415,8 +2490,11 @@
       <c r="P19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2424,7 +2502,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2470,8 +2548,11 @@
       <c r="P21" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2488,7 +2569,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2505,7 +2586,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2521,13 +2602,13 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="2">
-        <f>AVERAGE(D25:P25)</f>
-        <v>1.8653846153846152</v>
+        <f>AVERAGE(D25:Q25)</f>
+        <v>1.9535714285714285</v>
       </c>
       <c r="D25" s="2">
         <v>1.3</v>
@@ -2568,8 +2649,11 @@
       <c r="P25" s="2">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="2">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2577,7 +2661,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2613,8 +2697,11 @@
       <c r="P27" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
@@ -2647,8 +2734,11 @@
       <c r="P28" s="2">
         <v>381</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2686,8 +2776,12 @@
         <f t="shared" si="7"/>
         <v>415</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="2">
+        <f t="shared" ref="Q29" si="8">SUM(Q27:Q28)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2695,7 +2789,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2703,63 +2797,67 @@
         <v>21</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D31:P31)</f>
-        <v>0.34107315931958315</v>
+        <f>AVERAGE(D31:Q31)</f>
+        <v>0.35752711732736803</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:J31" si="8">(D18/D12)</f>
+        <f t="shared" ref="D31:J31" si="9">(D18/D12)</f>
         <v>0.40625</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.375</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31:L31" si="9">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="10">(K18/K12)</f>
         <v>0.375</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.26470588235294118</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ref="M31:N31" si="10">(M18/M12)</f>
+        <f t="shared" ref="M31:N31" si="11">(M18/M12)</f>
         <v>0.5</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.3888888888888889</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" ref="O31:P31" si="11">(O18/O12)</f>
+        <f t="shared" ref="O31:P31" si="12">(O18/O12)</f>
         <v>0.15151515151515152</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.5714285714285714</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="2">
+        <f t="shared" ref="Q31" si="13">(Q18/Q12)</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="B32" s="5" t="s">
         <v>28</v>
       </c>
@@ -2767,169 +2865,181 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="12">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="14">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32:L32" si="13">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="15">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32:N32" si="14">(M19/M12)</f>
+        <f t="shared" ref="M32:N32" si="16">(M19/M12)</f>
         <v>0.125</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" ref="O32:P32" si="15">(O19/O12)</f>
+        <f t="shared" ref="O32:P32" si="17">(O19/O12)</f>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.14285714285714285</v>
       </c>
-    </row>
-    <row r="33" spans="2:16">
+      <c r="Q32" s="2">
+        <f t="shared" ref="Q32" si="18">(Q19/Q12)</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D33:P33)</f>
-        <v>0.77090559204990983</v>
+        <f>AVERAGE(D33:Q33)</f>
+        <v>0.77536471642729732</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="16">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="19">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:L33" si="17">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="20">K17/K5</f>
         <v>0.875</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.95348837209302328</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33:N33" si="18">M17/M5</f>
+        <f t="shared" ref="M33:N33" si="21">M17/M5</f>
         <v>0.375</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>0.7</v>
       </c>
       <c r="O33" s="2">
-        <f t="shared" ref="O33:P33" si="19">O17/O5</f>
+        <f t="shared" ref="O33:P33" si="22">O17/O5</f>
         <v>1.0172413793103448</v>
       </c>
       <c r="P33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>0.82499999999999996</v>
       </c>
-    </row>
-    <row r="34" spans="2:16">
+      <c r="Q33" s="2">
+        <f t="shared" ref="Q33" si="23">Q17/Q5</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17">
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D34:P34)</f>
-        <v>0.59799108126379286</v>
+        <f>AVERAGE(D34:Q34)</f>
+        <v>0.57379595112061188</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="20">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="24">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34:L34" si="21">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="25">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0.79069767441860461</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34:N34" si="22">M12/M5</f>
+        <f t="shared" ref="M34:N34" si="26">M12/M5</f>
         <v>0.25</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="O34" s="2">
-        <f t="shared" ref="O34:P34" si="23">O12/O5</f>
+        <f t="shared" ref="O34:P34" si="27">O12/O5</f>
         <v>1.1379310344827587</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0.35</v>
       </c>
-    </row>
-    <row r="35" spans="2:16">
+      <c r="Q34" s="2">
+        <f t="shared" ref="Q34" si="28">Q12/Q5</f>
+        <v>0.25925925925925924</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17">
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -2946,139 +3056,154 @@
       <c r="P35" s="2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="37" spans="2:16">
+      <c r="Q35" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17">
       <c r="B37" s="5" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" ref="G37:L37" si="24">(G9/G12*100)</f>
+        <f t="shared" ref="G37:L37" si="29">(G9/G12*100)</f>
         <v>71.666666666666671</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>30.76923076923077</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>60</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>25.806451612903224</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>25</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ref="M37:N37" si="25">(M9/M12*100)</f>
+        <f t="shared" ref="M37:N37" si="30">(M9/M12*100)</f>
         <v>25</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>22.222222222222221</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" ref="O37:P37" si="26">(O9/O12*100)</f>
+        <f t="shared" ref="O37:P37" si="31">(O9/O12*100)</f>
         <v>66.666666666666657</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="38" spans="2:16">
+      <c r="Q37" s="2">
+        <f t="shared" ref="Q37" si="32">(Q9/Q12*100)</f>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17">
       <c r="B38" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ref="G38:L38" si="27">(G10/G12*100)</f>
+        <f t="shared" ref="G38:L38" si="33">(G10/G12*100)</f>
         <v>26.666666666666668</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>13.333333333333334</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>67.741935483870961</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>53.125</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" ref="M38:N38" si="28">(M10/M12*100)</f>
+        <f t="shared" ref="M38:N38" si="34">(M10/M12*100)</f>
         <v>75</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>77.777777777777786</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" ref="O38:P38" si="29">(O10/O12*100)</f>
+        <f t="shared" ref="O38:P38" si="35">(O10/O12*100)</f>
         <v>27.27272727272727</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>28.571428571428569</v>
       </c>
-    </row>
-    <row r="39" spans="2:16">
+      <c r="Q38" s="2">
+        <f t="shared" ref="Q38" si="36">(Q10/Q12*100)</f>
+        <v>71.428571428571431</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17">
       <c r="B39" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" ref="G39:L39" si="30">(G11/G12*100)</f>
+        <f t="shared" ref="G39:L39" si="37">(G11/G12*100)</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>26.666666666666668</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>6.4516129032258061</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>21.875</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>23.52941176470588</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" ref="M39:N39" si="31">(M11/M12*100)</f>
+        <f t="shared" ref="M39:N39" si="38">(M11/M12*100)</f>
         <v>0</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" ref="O39:P39" si="32">(O11/O12*100)</f>
+        <f t="shared" ref="O39:P39" si="39">(O11/O12*100)</f>
         <v>6.0606060606060606</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" ref="Q39" si="40">(Q11/Q12*100)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update statistics and insights until 09 JUN 2015
</commit_message>
<xml_diff>
--- a/statistics/statistics_cologne.xlsx
+++ b/statistics/statistics_cologne.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Zeitraum</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>08 APR - 28 APR</t>
+  </si>
+  <si>
+    <t>29 APR - 19 MAY</t>
+  </si>
+  <si>
+    <t>20 MAY - 08 JUN</t>
   </si>
 </sst>
 </file>
@@ -210,8 +216,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -347,7 +361,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="133">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -410,6 +424,10 @@
     <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -472,6 +490,10 @@
     <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -850,11 +872,11 @@
         <c:dropLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2124147016"/>
-        <c:axId val="2124152040"/>
+        <c:axId val="2115177960"/>
+        <c:axId val="2116665464"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2124147016"/>
+        <c:axId val="2115177960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,14 +905,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124152040"/>
+        <c:crossAx val="2116665464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2124152040"/>
+        <c:axId val="2116665464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124147016"/>
+        <c:crossAx val="2115177960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1130,11 +1152,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2124191208"/>
-        <c:axId val="2124194088"/>
+        <c:axId val="2115154232"/>
+        <c:axId val="2115151192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2124191208"/>
+        <c:axId val="2115154232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,7 +1165,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124194088"/>
+        <c:crossAx val="2115151192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1151,7 +1173,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2124194088"/>
+        <c:axId val="2115151192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124191208"/>
+        <c:crossAx val="2115154232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1262,7 +1284,7 @@
           <a:fld id="{0D984E82-241E-B040-9441-E77404260ED3}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,78</a:t>
+            <a:t>0,77</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1316,7 +1338,7 @@
           <a:fld id="{E5687BA9-F129-9348-BC57-1C2935757FF8}" type="TxLink">
             <a:rPr lang="de-DE" sz="1100" b="1"/>
             <a:pPr/>
-            <a:t>0,57</a:t>
+            <a:t>0,61</a:t>
           </a:fld>
           <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
         </a:p>
@@ -1785,10 +1807,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="26" topLeftCell="P27" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1799,10 +1824,10 @@
     <col min="10" max="10" width="13.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
     <col min="12" max="14" width="13.83203125" style="2" customWidth="1"/>
-    <col min="15" max="17" width="14.33203125" style="2" customWidth="1"/>
+    <col min="15" max="19" width="14.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1851,8 +1876,14 @@
       <c r="Q1" s="1">
         <v>42123</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1">
+        <v>42143</v>
+      </c>
+      <c r="S1" s="1">
+        <v>42164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1898,8 +1929,14 @@
       <c r="Q2" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1907,7 +1944,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1954,8 +1991,14 @@
       <c r="Q4" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="2">
+        <v>13</v>
+      </c>
+      <c r="S4" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2002,8 +2045,14 @@
       <c r="Q5" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" s="2">
+        <v>17</v>
+      </c>
+      <c r="S5" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2011,7 +2060,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2022,7 +2071,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2030,7 +2079,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2073,8 +2122,14 @@
       <c r="Q9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" s="2">
+        <v>8</v>
+      </c>
+      <c r="S9" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
@@ -2114,8 +2169,14 @@
       <c r="Q10" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10" s="2">
+        <v>7</v>
+      </c>
+      <c r="S10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
@@ -2155,8 +2216,14 @@
       <c r="Q11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -2213,8 +2280,16 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" s="2">
+        <f t="shared" ref="R12:S12" si="3">SUM(R9:R11)</f>
+        <v>15</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -2222,7 +2297,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2265,8 +2340,14 @@
       <c r="Q14" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="S14" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
@@ -2306,8 +2387,14 @@
       <c r="Q15" s="2">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="R15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="S15" s="2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
@@ -2347,8 +2434,14 @@
       <c r="Q16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R16" s="2">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2362,51 +2455,59 @@
         <v>33.5</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" ref="G17:M17" si="3">SUM(G14:G16)</f>
+        <f t="shared" ref="G17:M17" si="4">SUM(G14:G16)</f>
         <v>54.5</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.5</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>41</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="N17" s="2">
-        <f t="shared" ref="N17:O17" si="4">SUM(N14:N16)</f>
+        <f t="shared" ref="N17:O17" si="5">SUM(N14:N16)</f>
         <v>24.5</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.5</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" ref="P17:Q17" si="5">SUM(P14:P16)</f>
+        <f t="shared" ref="P17:Q17" si="6">SUM(P14:P16)</f>
         <v>16.5</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="R17" s="2">
+        <f t="shared" ref="R17:S17" si="7">SUM(R14:R16)</f>
+        <v>14</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
@@ -2452,8 +2553,14 @@
       <c r="Q18" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="R18" s="2">
+        <v>0</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
@@ -2493,8 +2600,14 @@
       <c r="Q19" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="R19" s="2">
+        <v>1</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -2502,7 +2615,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2551,8 +2664,14 @@
       <c r="Q21" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="R21" s="2">
+        <v>2</v>
+      </c>
+      <c r="S21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
@@ -2569,7 +2688,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:19">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
@@ -2585,8 +2704,11 @@
       <c r="I23" s="4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="S23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2602,7 +2724,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:19">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
@@ -2652,8 +2774,14 @@
       <c r="Q25" s="2">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="R25" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="S25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
@@ -2661,7 +2789,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2700,8 +2828,14 @@
       <c r="Q27" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27" s="2">
+        <v>37</v>
+      </c>
+      <c r="S27" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="B28" s="5" t="s">
         <v>12</v>
       </c>
@@ -2737,51 +2871,65 @@
       <c r="Q28" s="2">
         <v>382</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="R28" s="2">
+        <v>382</v>
+      </c>
+      <c r="S28" s="2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2">
-        <f t="shared" ref="I29:N29" si="6">SUM(I27:I28)</f>
+        <f t="shared" ref="I29:N29" si="8">SUM(I27:I28)</f>
         <v>317</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>325</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>338</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>338</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>369</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>387</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" ref="O29:P29" si="7">SUM(O27:O28)</f>
+        <f t="shared" ref="O29:P29" si="9">SUM(O27:O28)</f>
         <v>409</v>
       </c>
       <c r="P29" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>415</v>
       </c>
       <c r="Q29" s="2">
-        <f t="shared" ref="Q29" si="8">SUM(Q27:Q28)</f>
+        <f t="shared" ref="Q29:R29" si="10">SUM(Q27:Q28)</f>
         <v>420</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="R29" s="2">
+        <f t="shared" si="10"/>
+        <v>419</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" ref="S29" si="11">SUM(S27:S28)</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2789,7 +2937,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2797,253 +2945,292 @@
         <v>21</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D31:Q31)</f>
-        <v>0.35752711732736803</v>
+        <f>AVERAGE(D31:S31)</f>
+        <v>0.31283622766144703</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" ref="D31:J31" si="9">(D18/D12)</f>
+        <f t="shared" ref="D31:J31" si="12">(D18/D12)</f>
         <v>0.40625</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.375</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.11666666666666667</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.38461538461538464</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.22580645161290322</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" ref="K31:L31" si="10">(K18/K12)</f>
+        <f t="shared" ref="K31:L31" si="13">(K18/K12)</f>
         <v>0.375</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.26470588235294118</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ref="M31:N31" si="11">(M18/M12)</f>
+        <f t="shared" ref="M31:N31" si="14">(M18/M12)</f>
         <v>0.5</v>
       </c>
       <c r="N31" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.3888888888888889</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" ref="O31:P31" si="12">(O18/O12)</f>
+        <f t="shared" ref="O31:P31" si="15">(O18/O12)</f>
         <v>0.15151515151515152</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="Q31" s="2">
-        <f t="shared" ref="Q31" si="13">(Q18/Q12)</f>
+        <f t="shared" ref="Q31:R31" si="16">(Q18/Q12)</f>
         <v>0.5714285714285714</v>
       </c>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="R31" s="2">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" ref="S31" si="17">(S18/S12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="B32" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="C32" s="2">
+        <f>AVERAGE(G32:S32)</f>
+        <v>8.8009731575451902E-2</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" ref="G32:J32" si="14">(G19/G12)</f>
+        <f t="shared" ref="G32:J32" si="18">(G19/G12)</f>
         <v>0.05</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.11538461538461539</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>6.4516129032258063E-2</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" ref="K32:L32" si="15">(K19/K12)</f>
+        <f t="shared" ref="K32:L32" si="19">(K19/K12)</f>
         <v>9.375E-2</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32:N32" si="16">(M19/M12)</f>
+        <f t="shared" ref="M32:N32" si="20">(M19/M12)</f>
         <v>0.125</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" ref="O32:P32" si="17">(O19/O12)</f>
+        <f t="shared" ref="O32:P32" si="21">(O19/O12)</f>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="Q32" s="2">
-        <f t="shared" ref="Q32" si="18">(Q19/Q12)</f>
+        <f t="shared" ref="Q32:R32" si="22">(Q19/Q12)</f>
         <v>0.2857142857142857</v>
       </c>
-    </row>
-    <row r="33" spans="2:17">
+      <c r="R32" s="2">
+        <f t="shared" si="22"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" ref="S32" si="23">(S19/S12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19">
       <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D33:Q33)</f>
-        <v>0.77536471642729732</v>
+        <f>AVERAGE(D33:S33)</f>
+        <v>0.76637304844251264</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" ref="D33:J33" si="19">D17/D5</f>
+        <f t="shared" ref="D33:J33" si="24">D17/D5</f>
         <v>0.75862068965517238</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>1.1551724137931034</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.63372093023255816</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.76530612244897955</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.5</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>0.69791666666666663</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" ref="K33:L33" si="20">K17/K5</f>
+        <f t="shared" ref="K33:L33" si="25">K17/K5</f>
         <v>0.875</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.95348837209302328</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33:N33" si="21">M17/M5</f>
+        <f t="shared" ref="M33:N33" si="26">M17/M5</f>
         <v>0.375</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.7</v>
       </c>
       <c r="O33" s="2">
-        <f t="shared" ref="O33:P33" si="22">O17/O5</f>
+        <f t="shared" ref="O33:P33" si="27">O17/O5</f>
         <v>1.0172413793103448</v>
       </c>
       <c r="P33" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>0.82499999999999996</v>
       </c>
       <c r="Q33" s="2">
-        <f t="shared" ref="Q33" si="23">Q17/Q5</f>
+        <f t="shared" ref="Q33:R33" si="28">Q17/Q5</f>
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="34" spans="2:17">
+      <c r="R33" s="2">
+        <f t="shared" si="28"/>
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" ref="S33" si="29">S17/S5</f>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19">
       <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D34:Q34)</f>
-        <v>0.57379595112061188</v>
+        <f>AVERAGE(D34:S34)</f>
+        <v>0.61190601605406481</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" ref="D34:J34" si="24">D12/D5</f>
+        <f t="shared" ref="D34:J34" si="30">D12/D5</f>
         <v>0.55172413793103448</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.55102040816326525</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.55172413793103448</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.69767441860465118</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.53061224489795922</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.5357142857142857</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34:L34" si="25">K12/K5</f>
+        <f t="shared" ref="K34:L34" si="31">K12/K5</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>0.79069767441860461</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34:N34" si="26">M12/M5</f>
+        <f t="shared" ref="M34:N34" si="32">M12/M5</f>
         <v>0.25</v>
       </c>
       <c r="N34" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="32"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="O34" s="2">
-        <f t="shared" ref="O34:P34" si="27">O12/O5</f>
+        <f t="shared" ref="O34:P34" si="33">O12/O5</f>
         <v>1.1379310344827587</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="33"/>
         <v>0.35</v>
       </c>
       <c r="Q34" s="2">
-        <f t="shared" ref="Q34" si="28">Q12/Q5</f>
+        <f t="shared" ref="Q34:R34" si="34">Q12/Q5</f>
         <v>0.25925925925925924</v>
       </c>
-    </row>
-    <row r="35" spans="2:17">
+      <c r="R34" s="2">
+        <f t="shared" si="34"/>
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" ref="S34" si="35">S12/S5</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19">
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2">
+        <f>AVERAGE(O35:S35)</f>
+        <v>2.9</v>
+      </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -3059,151 +3246,181 @@
       <c r="Q35" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="2:17">
+      <c r="R35" s="2">
+        <v>3</v>
+      </c>
+      <c r="S35" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19">
       <c r="B37" s="5" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" ref="G37:L37" si="29">(G9/G12*100)</f>
+        <f t="shared" ref="G37:L37" si="36">(G9/G12*100)</f>
         <v>71.666666666666671</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>30.76923076923077</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>60</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>25.806451612903224</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>25</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ref="M37:N37" si="30">(M9/M12*100)</f>
+        <f t="shared" ref="M37:N37" si="37">(M9/M12*100)</f>
         <v>25</v>
       </c>
       <c r="N37" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>22.222222222222221</v>
       </c>
       <c r="O37" s="2">
-        <f t="shared" ref="O37:P37" si="31">(O9/O12*100)</f>
+        <f t="shared" ref="O37:P37" si="38">(O9/O12*100)</f>
         <v>66.666666666666657</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>71.428571428571431</v>
       </c>
       <c r="Q37" s="2">
-        <f t="shared" ref="Q37" si="32">(Q9/Q12*100)</f>
+        <f t="shared" ref="Q37:R37" si="39">(Q9/Q12*100)</f>
         <v>28.571428571428569</v>
       </c>
-    </row>
-    <row r="38" spans="2:17">
+      <c r="R37" s="2">
+        <f t="shared" si="39"/>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" ref="S37" si="40">(S9/S12*100)</f>
+        <v>52.380952380952387</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19">
       <c r="B38" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" ref="G38:L38" si="33">(G10/G12*100)</f>
+        <f t="shared" ref="G38:L38" si="41">(G10/G12*100)</f>
         <v>26.666666666666668</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>13.333333333333334</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>67.741935483870961</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>53.125</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>38.235294117647058</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" ref="M38:N38" si="34">(M10/M12*100)</f>
+        <f t="shared" ref="M38:N38" si="42">(M10/M12*100)</f>
         <v>75</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>77.777777777777786</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" ref="O38:P38" si="35">(O10/O12*100)</f>
+        <f t="shared" ref="O38:P38" si="43">(O10/O12*100)</f>
         <v>27.27272727272727</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>28.571428571428569</v>
       </c>
       <c r="Q38" s="2">
-        <f t="shared" ref="Q38" si="36">(Q10/Q12*100)</f>
+        <f t="shared" ref="Q38:R38" si="44">(Q10/Q12*100)</f>
         <v>71.428571428571431</v>
       </c>
-    </row>
-    <row r="39" spans="2:17">
+      <c r="R38" s="2">
+        <f t="shared" si="44"/>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" ref="S38" si="45">(S10/S12*100)</f>
+        <v>47.619047619047613</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19">
       <c r="B39" s="5" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" ref="G39:L39" si="37">(G11/G12*100)</f>
+        <f t="shared" ref="G39:L39" si="46">(G11/G12*100)</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="46"/>
         <v>34.615384615384613</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="46"/>
         <v>26.666666666666668</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="46"/>
         <v>6.4516129032258061</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="46"/>
         <v>21.875</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="46"/>
         <v>23.52941176470588</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" ref="M39:N39" si="38">(M11/M12*100)</f>
+        <f t="shared" ref="M39:N39" si="47">(M11/M12*100)</f>
         <v>0</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" ref="O39:P39" si="39">(O11/O12*100)</f>
+        <f t="shared" ref="O39:P39" si="48">(O11/O12*100)</f>
         <v>6.0606060606060606</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="Q39" s="2">
-        <f t="shared" ref="Q39" si="40">(Q11/Q12*100)</f>
+        <f t="shared" ref="Q39:R39" si="49">(Q11/Q12*100)</f>
+        <v>0</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" ref="S39" si="50">(S11/S12*100)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>